<commit_message>
changes in BOM orders
</commit_message>
<xml_diff>
--- a/BLE_sensors_pcb/BOM/BLE_sensors_BOM.xlsx
+++ b/BLE_sensors_pcb/BOM/BLE_sensors_BOM.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Desktop\Files\School\Thesis\BLE_sensors\BLE_sensors_pcb\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vasiloglou\Desktop\Work_Files\BLE_sensors\BLE_sensors_pcb\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDC63589-E207-4AD8-8F37-C345D54A15B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51600" windowHeight="17730"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Φύλλο1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="71">
   <si>
     <t>Reference</t>
   </si>
@@ -36,9 +37,6 @@
   </si>
   <si>
     <t>Footprint</t>
-  </si>
-  <si>
-    <t>DNP</t>
   </si>
   <si>
     <t>Ordered</t>
@@ -245,7 +243,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -309,7 +307,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Κανονικό" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -586,22 +584,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="64.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="68.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -620,455 +618,438 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="B2" s="1">
         <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1">
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="1">
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="1">
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" s="1">
         <v>3</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="1">
-        <v>1</v>
-      </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="1">
-        <v>1</v>
-      </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="1">
-        <v>1</v>
-      </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
+      <c r="B11" s="1">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="1">
-        <v>1</v>
-      </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B12" s="1">
         <v>2</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="1">
-        <v>1</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="D13" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="1">
-        <v>1</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="D14" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B15" s="1">
         <v>3</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B16" s="1">
         <v>2</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B17" s="1">
         <v>2</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B18" s="1">
         <v>2</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" s="1">
+        <v>1</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="1">
-        <v>1</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="D19" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B20" s="1">
         <v>2</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B21" s="1">
         <v>4</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" s="1">
+        <v>1</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B22" s="1">
-        <v>1</v>
-      </c>
-      <c r="C22" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="E22" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A23" s="1" t="s">
+      <c r="B23" s="1">
+        <v>1</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B23" s="1">
-        <v>1</v>
-      </c>
-      <c r="C23" s="1" t="s">
+      <c r="D23" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="E23" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A24" s="1" t="s">
+      <c r="B24" s="1">
+        <v>1</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B24" s="1">
-        <v>1</v>
-      </c>
-      <c r="C24" s="1" t="s">
+      <c r="D24" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="E24" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F24" s="1"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A25" s="1" t="s">
+      <c r="B25" s="1">
+        <v>1</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B25" s="1">
-        <v>1</v>
-      </c>
-      <c r="C25" s="1" t="s">
+      <c r="D25" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="E25" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E25" s="1"/>
       <c r="F25" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="G25" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A26" s="1" t="s">
+      <c r="B26" s="1">
+        <v>1</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B26" s="1">
-        <v>1</v>
-      </c>
-      <c r="C26" s="1" t="s">
+      <c r="D26" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="E26" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F26" s="1"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A27" s="1" t="s">
+      <c r="B27" s="1">
+        <v>1</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B27" s="1">
-        <v>1</v>
-      </c>
-      <c r="C27" s="1" t="s">
+      <c r="D27" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D27" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E27" s="1"/>
+      <c r="E27" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>